<commit_message>
Added validations for Sort and Filter in results page
</commit_message>
<xml_diff>
--- a/src/test/resources/data/sample.xlsx
+++ b/src/test/resources/data/sample.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="195">
   <si>
     <t>MailID</t>
   </si>
@@ -454,9 +454,6 @@
     <t>Accommodation|Activities of extraterritorial organisations and bodies|Administrative and support service activities|Agriculture, forestry and fishing|Arts, entertainment and recreation|Construction|Education|Electricity, gas, steam and air conditioning supply|Financial and insurance activities|Human health and social work activities|Information and communication|Manufacturing|Mining and quarrying|Professional, scientific and technical activities|Public administrative and defence; compulsory social security|Real estate activities|Transportation and storage|Undifferentiated goods and services-producing activities of households for own use|Water supply; sewerage, waste management and remediation activities|Wholesale and retail trade; repair of motor vehicles and motorcycles|</t>
   </si>
   <si>
-    <t>Direct Grant|Equity|Guarantee|Loan|Purchase of goods or services above market prices|Sale of goods or services below market prices|Tax measures (tax credit, or tax/duty exemption)|Other|</t>
-  </si>
-  <si>
     <t>USTD_015</t>
   </si>
   <si>
@@ -466,9 +463,6 @@
     <t>Training|Energy efficiency|Rescue aid</t>
   </si>
   <si>
-    <t>Culture/Heritage|Employment|Energy efficiency|Environmental protection|Infrastructure|Regional development|Rescue aid|Research and development|SME (Small/Medium-sized enterprise) support|Training|Other|</t>
-  </si>
-  <si>
     <t>Belfast Health Trust|SELFRIDGE LTD|Mr Robert Smith|EasyJet LTD</t>
   </si>
   <si>
@@ -599,6 +593,42 @@
   </si>
   <si>
     <t>Date|DSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research and development|SME (Small/Medium-sized enterprise) </t>
+  </si>
+  <si>
+    <t>Agriculture, forestry and fishing|Arts, entertainment and recreation</t>
+  </si>
+  <si>
+    <t>Other Purpose Filter</t>
+  </si>
+  <si>
+    <t>Other Type Filter</t>
+  </si>
+  <si>
+    <t>Culture/Heritage|Employment|Energy efficiency|Environmental protection|Infrastructure|Regional development|Rescue aid|Research and development|SME (Small/Medium-sized enterprise) support|Training|</t>
+  </si>
+  <si>
+    <t>Direct Grant|Equity|Guarantee|Loan|Purchase of goods or services above market prices|Sale of goods or services below market prices|Tax measures (tax credit, or tax/duty exemption)</t>
+  </si>
+  <si>
+    <t>USTD_029</t>
+  </si>
+  <si>
+    <t>Durham Medical Trust|RyanAir LTD|Seed Animation Limited|Mr Ben Stokes|Western Ferries (Clyde) Limited|Belfast Health Trust|SELFRIDGE LTD|DS SMITH PAPER LIMITED|ITV LTD|Mr Robert Smith|EasyJet LTD|</t>
+  </si>
+  <si>
+    <t>Select all|Select all|Accommodation|Activities of extraterritorial organisations and bodies|Administrative and support service activities|Agriculture, forestry and fishing|Arts, entertainment and recreation|Construction|Education|Electricity, gas, steam and air conditioning supply|Financial and insurance activities|Human health and social work activities|Information and communication|Manufacturing|Mining and quarrying|Professional, scientific and technical activities|Public administrative and defence; compulsory social security|Real estate activities|Transportation and storage|Undifferentiated goods and services-producing activities of households for own use|Water supply; sewerage, waste management and remediation activities|Wholesale and retail trade; repair of motor vehicles and motorcycles|</t>
+  </si>
+  <si>
+    <t>Select all|Direct Grant|Equity|Guarantee|Loan|Purchase of goods or services above market prices|Sale of goods or services below market prices|Tax measures (tax credit, or tax/duty exemption)|Other|Other</t>
+  </si>
+  <si>
+    <t>Select all|Culture/Heritage|Employment|Energy efficiency|Environmental protection|Infrastructure|Regional development|Rescue aid|Research and development|SME (Small/Medium-sized enterprise) support|Training|Other|</t>
+  </si>
+  <si>
+    <t>Other|</t>
   </si>
 </sst>
 </file>
@@ -681,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -730,6 +760,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1592,10 +1625,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:X48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1609,88 +1644,94 @@
     <col min="7" max="7" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="19.7265625" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="75.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.7265625" customWidth="1"/>
+    <col min="10" max="14" width="19.7265625" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="75.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="O1" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="F1" s="21" t="s">
+      <c r="P1" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q1" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="H1" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="L1" s="21" t="s">
+      <c r="S1" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="X1" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="M1" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q1" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="S1" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="T1" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="U1" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="V1" s="21" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>102</v>
       </c>
@@ -1705,22 +1746,24 @@
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
-      <c r="M2" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N2" s="12" t="s">
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P2" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
       <c r="T2" s="15"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="13"/>
-    </row>
-    <row r="3" spans="1:22" ht="261" x14ac:dyDescent="0.35">
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="13"/>
+    </row>
+    <row r="3" spans="1:24" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>103</v>
       </c>
@@ -1728,16 +1771,16 @@
         <v>107</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>140</v>
+        <v>194</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>105</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>135</v>
+        <v>191</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>136</v>
+        <v>192</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>106</v>
@@ -1748,28 +1791,34 @@
       <c r="I3" s="13">
         <v>42231</v>
       </c>
-      <c r="J3" s="13"/>
+      <c r="J3" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
+      <c r="L3" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="P3" s="12"/>
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
       <c r="S3" s="15"/>
       <c r="T3" s="15"/>
       <c r="U3" s="15"/>
-      <c r="V3" s="13"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="13"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>104</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
@@ -1781,28 +1830,30 @@
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
       <c r="L4" s="16"/>
-      <c r="M4" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>141</v>
+      </c>
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
       <c r="U4" s="15"/>
-      <c r="V4" s="16"/>
-    </row>
-    <row r="5" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="16"/>
+    </row>
+    <row r="5" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>121</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -1813,22 +1864,24 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
-      <c r="M5" s="20" t="s">
-        <v>153</v>
-      </c>
+      <c r="M5" s="16"/>
       <c r="N5" s="16"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="17" t="s">
-        <v>139</v>
-      </c>
+      <c r="O5" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
+      <c r="S5" s="17" t="s">
+        <v>138</v>
+      </c>
       <c r="T5" s="15"/>
       <c r="U5" s="15"/>
-      <c r="V5" s="16"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="16"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>122</v>
       </c>
@@ -1847,22 +1900,24 @@
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
       <c r="L6" s="16"/>
-      <c r="M6" s="20" t="s">
-        <v>153</v>
-      </c>
+      <c r="M6" s="16"/>
       <c r="N6" s="16"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="16" t="s">
+      <c r="O6" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
       <c r="T6" s="15"/>
       <c r="U6" s="15"/>
-      <c r="V6" s="16"/>
-    </row>
-    <row r="7" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="16"/>
+    </row>
+    <row r="7" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>123</v>
       </c>
@@ -1879,22 +1934,24 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
       <c r="L7" s="16"/>
-      <c r="M7" s="20" t="s">
-        <v>144</v>
-      </c>
+      <c r="M7" s="16"/>
       <c r="N7" s="16"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
+      <c r="O7" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P7" s="16"/>
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
-      <c r="S7" s="12" t="s">
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="16"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="16"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>124</v>
       </c>
@@ -1911,22 +1968,24 @@
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
-      <c r="M8" s="19" t="s">
-        <v>155</v>
-      </c>
+      <c r="M8" s="16"/>
       <c r="N8" s="16"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
+      <c r="O8" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="P8" s="16"/>
       <c r="Q8" s="15"/>
-      <c r="R8" s="15" t="s">
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
       <c r="U8" s="15"/>
-      <c r="V8" s="16"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="16"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>125</v>
       </c>
@@ -1945,22 +2004,24 @@
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
-      <c r="M9" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="N9" s="14"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="P9" s="14"/>
       <c r="Q9" s="15"/>
-      <c r="R9" s="15" t="s">
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
       <c r="U9" s="15"/>
-      <c r="V9" s="12"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="12"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>126</v>
       </c>
@@ -1979,24 +2040,26 @@
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
-      <c r="M10" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="N10" s="14"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="P10" s="14"/>
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
       <c r="S10" s="15"/>
-      <c r="T10" s="13">
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="13">
         <v>43101</v>
       </c>
-      <c r="U10" s="13">
+      <c r="W10" s="13">
         <v>43831</v>
       </c>
-      <c r="V10" s="13"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X10" s="13"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>127</v>
       </c>
@@ -2021,24 +2084,26 @@
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
-      <c r="M11" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N11" s="12" t="s">
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P11" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15" t="s">
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
-      <c r="V11" s="12"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="12"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>128</v>
       </c>
@@ -2065,22 +2130,24 @@
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
-      <c r="M12" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N12" s="12" t="s">
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P12" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
       <c r="S12" s="15"/>
       <c r="T12" s="15"/>
       <c r="U12" s="15"/>
-      <c r="V12" s="12"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="12"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>129</v>
       </c>
@@ -2107,22 +2174,24 @@
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
-      <c r="M13" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N13" s="12" t="s">
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P13" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
       <c r="S13" s="15"/>
       <c r="T13" s="15"/>
       <c r="U13" s="15"/>
-      <c r="V13" s="13"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="13"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>130</v>
       </c>
@@ -2149,22 +2218,24 @@
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
-      <c r="M14" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N14" s="12" t="s">
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P14" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="15"/>
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
       <c r="U14" s="15"/>
-      <c r="V14" s="12"/>
-    </row>
-    <row r="15" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="12"/>
+    </row>
+    <row r="15" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>131</v>
       </c>
@@ -2191,24 +2262,26 @@
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
-      <c r="M15" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N15" s="12" t="s">
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P15" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
       <c r="R15" s="15"/>
       <c r="S15" s="15"/>
       <c r="T15" s="15"/>
       <c r="U15" s="15"/>
-      <c r="V15" s="13"/>
-    </row>
-    <row r="16" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="13"/>
+    </row>
+    <row r="16" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>100</v>
@@ -2233,24 +2306,26 @@
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
-      <c r="M16" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N16" s="12" t="s">
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P16" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
       <c r="Q16" s="15"/>
       <c r="R16" s="15"/>
       <c r="S16" s="15"/>
       <c r="T16" s="15"/>
       <c r="U16" s="15"/>
-      <c r="V16" s="12"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="12"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
@@ -2273,24 +2348,26 @@
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
-      <c r="M17" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N17" s="12" t="s">
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P17" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
       <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
       <c r="S17" s="15"/>
       <c r="T17" s="15"/>
       <c r="U17" s="15"/>
-      <c r="V17" s="13"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="13"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
@@ -2313,24 +2390,26 @@
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
-      <c r="M18" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N18" s="12" t="s">
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P18" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
       <c r="S18" s="15"/>
       <c r="T18" s="15"/>
       <c r="U18" s="15"/>
-      <c r="V18" s="12"/>
-    </row>
-    <row r="19" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="12"/>
+    </row>
+    <row r="19" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12" t="s">
@@ -2353,24 +2432,26 @@
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
-      <c r="M19" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N19" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P19" s="12" t="s">
+        <v>139</v>
+      </c>
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
       <c r="S19" s="15"/>
       <c r="T19" s="15"/>
       <c r="U19" s="15"/>
-      <c r="V19" s="13"/>
-    </row>
-    <row r="20" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="13"/>
+    </row>
+    <row r="20" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12" t="s">
@@ -2393,24 +2474,26 @@
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
-      <c r="M20" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N20" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>139</v>
+      </c>
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
       <c r="S20" s="15"/>
       <c r="T20" s="15"/>
       <c r="U20" s="15"/>
-      <c r="V20" s="12"/>
-    </row>
-    <row r="21" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="12"/>
+    </row>
+    <row r="21" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12" t="s">
@@ -2433,24 +2516,26 @@
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
-      <c r="M21" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N21" s="14" t="s">
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P21" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
       <c r="S21" s="15"/>
       <c r="T21" s="15"/>
       <c r="U21" s="15"/>
-      <c r="V21" s="12"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="12"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="12"/>
@@ -2465,24 +2550,26 @@
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
-      <c r="M22" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="N22" s="14"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="P22" s="14"/>
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
       <c r="S22" s="15"/>
-      <c r="T22" s="13">
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="13">
         <v>43101</v>
       </c>
-      <c r="U22" s="12"/>
-      <c r="V22" s="12"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W22" s="12"/>
+      <c r="X22" s="12"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="12"/>
@@ -2497,24 +2584,26 @@
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
-      <c r="M23" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="N23" s="14"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="P23" s="14"/>
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
       <c r="S23" s="15"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13">
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13">
         <v>44197</v>
       </c>
-      <c r="V23" s="13"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X23" s="13"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -2527,24 +2616,26 @@
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
       <c r="L24" s="16"/>
-      <c r="M24" s="19" t="s">
-        <v>171</v>
-      </c>
+      <c r="M24" s="16"/>
       <c r="N24" s="16"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
+      <c r="O24" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="P24" s="16"/>
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
       <c r="U24" s="15"/>
-      <c r="V24" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -2557,24 +2648,26 @@
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
       <c r="L25" s="16"/>
-      <c r="M25" s="19" t="s">
-        <v>171</v>
-      </c>
+      <c r="M25" s="16"/>
       <c r="N25" s="16"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
+      <c r="O25" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="P25" s="16"/>
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
       <c r="S25" s="15"/>
       <c r="T25" s="15"/>
       <c r="U25" s="15"/>
-      <c r="V25" s="16" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V25" s="15"/>
+      <c r="W25" s="15"/>
+      <c r="X25" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -2587,24 +2680,26 @@
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
       <c r="L26" s="16"/>
-      <c r="M26" s="19" t="s">
-        <v>171</v>
-      </c>
+      <c r="M26" s="16"/>
       <c r="N26" s="16"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
+      <c r="O26" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="P26" s="16"/>
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
       <c r="S26" s="15"/>
       <c r="T26" s="15"/>
       <c r="U26" s="15"/>
-      <c r="V26" s="16" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V26" s="15"/>
+      <c r="W26" s="15"/>
+      <c r="X26" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -2617,24 +2712,26 @@
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
       <c r="L27" s="16"/>
-      <c r="M27" s="19" t="s">
-        <v>171</v>
-      </c>
+      <c r="M27" s="16"/>
       <c r="N27" s="16"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
+      <c r="O27" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="P27" s="16"/>
       <c r="Q27" s="15"/>
       <c r="R27" s="15"/>
       <c r="S27" s="15"/>
       <c r="T27" s="15"/>
       <c r="U27" s="15"/>
-      <c r="V27" s="16" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V27" s="15"/>
+      <c r="W27" s="15"/>
+      <c r="X27" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -2647,24 +2744,26 @@
       <c r="J28" s="16"/>
       <c r="K28" s="16"/>
       <c r="L28" s="16"/>
-      <c r="M28" s="19" t="s">
-        <v>171</v>
-      </c>
+      <c r="M28" s="16"/>
       <c r="N28" s="16"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
+      <c r="O28" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="P28" s="16"/>
       <c r="Q28" s="15"/>
       <c r="R28" s="15"/>
       <c r="S28" s="15"/>
       <c r="T28" s="15"/>
       <c r="U28" s="15"/>
-      <c r="V28" s="16" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V28" s="15"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -2677,23 +2776,27 @@
       <c r="J29" s="16"/>
       <c r="K29" s="16"/>
       <c r="L29" s="16"/>
-      <c r="M29" s="19" t="s">
-        <v>171</v>
-      </c>
+      <c r="M29" s="16"/>
       <c r="N29" s="16"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
+      <c r="O29" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="P29" s="16"/>
       <c r="Q29" s="15"/>
       <c r="R29" s="15"/>
       <c r="S29" s="15"/>
       <c r="T29" s="15"/>
       <c r="U29" s="15"/>
-      <c r="V29" s="16" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A30" s="8"/>
+      <c r="V29" s="15"/>
+      <c r="W29" s="15"/>
+      <c r="X29" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
+        <v>189</v>
+      </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -2702,17 +2805,35 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="V30" s="8"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="J30" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="O30" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="P30" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="X30" s="8"/>
+    </row>
+    <row r="31" spans="1:24" ht="174" x14ac:dyDescent="0.35">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
+      <c r="C31" s="23" t="s">
+        <v>193</v>
+      </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
@@ -2724,9 +2845,13 @@
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
-      <c r="V31" s="8"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O31" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="P31" s="8"/>
+      <c r="X31" s="8"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -2741,9 +2866,13 @@
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
-      <c r="V32" s="8"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O32" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="P32" s="8"/>
+      <c r="X32" s="8"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2758,9 +2887,11 @@
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
-      <c r="V33" s="8"/>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="X33" s="8"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -2775,9 +2906,11 @@
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
-      <c r="V34" s="8"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="X34" s="8"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -2792,9 +2925,11 @@
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
-      <c r="V35" s="8"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="X35" s="8"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -2809,9 +2944,11 @@
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
-      <c r="V36" s="8"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="X36" s="8"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -2826,9 +2963,11 @@
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
-      <c r="V37" s="8"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="X37" s="8"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -2843,9 +2982,11 @@
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
-      <c r="V38" s="8"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="X38" s="8"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -2860,9 +3001,11 @@
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
-      <c r="V39" s="8"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="X39" s="8"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -2877,9 +3020,11 @@
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
-      <c r="V40" s="8"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="X40" s="8"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -2894,9 +3039,11 @@
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
-      <c r="V41" s="8"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="X41" s="8"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -2911,9 +3058,11 @@
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
-      <c r="V42" s="8"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="X42" s="8"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -2928,9 +3077,11 @@
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
-      <c r="V43" s="8"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="X43" s="8"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -2945,9 +3096,11 @@
       <c r="L44" s="8"/>
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
-      <c r="V44" s="8"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="X44" s="8"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -2962,9 +3115,11 @@
       <c r="L45" s="8"/>
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
-      <c r="V45" s="8"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="X45" s="8"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -2979,9 +3134,11 @@
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
-      <c r="V46" s="8"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="X46" s="8"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -2996,9 +3153,11 @@
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
       <c r="N47" s="8"/>
-      <c r="V47" s="8"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="X47" s="8"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -3012,10 +3171,12 @@
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
-      <c r="V48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="X48" s="8"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" showErrorMessage="1" errorTitle="Automation" error="Do not change the Column header name as this will break Automation scripts" prompt="Do not change the Column Header Values" sqref="B1">
       <formula1>"Recipient"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
API automation changes 14th Jan
</commit_message>
<xml_diff>
--- a/src/test/resources/data/sample.xlsx
+++ b/src/test/resources/data/sample.xlsx
@@ -18,7 +18,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="240">
   <si>
     <t>MailID</t>
   </si>
@@ -766,12 +766,16 @@
   </si>
   <si>
     <t>Almond Valley Heritage Trust</t>
+  </si>
+  <si>
+    <t>Monetise International Ltd|MR THOMAS (JUN) OBRIEN|DS SMITH PAPER LIMITED 100|DS SMITH PAPER LIMITED 100|Jonathan|Peter|Daria|Terelak</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1203,9 +1207,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.08984375" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.1796875" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.81640625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1277,21 +1281,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" customWidth="1"/>
-    <col min="4" max="4" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.1796875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="13.90625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="22.1796875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.36328125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="42.54296875" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.08984375" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="31.0" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="26.7265625" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.6328125" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="27.1796875" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="20.81640625" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="46.1796875" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="17.36328125" collapsed="false"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="15.6328125" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="26.26953125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
@@ -1779,33 +1783,33 @@
   <dimension ref="A1:X54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="19.7265625" customWidth="1"/>
-    <col min="15" max="15" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="75.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.7265625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.6328125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.90625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.26953125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1796875" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="45.6328125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.26953125" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.54296875" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.08984375" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="19.7265625" collapsed="false"/>
+    <col min="10" max="14" customWidth="true" width="19.7265625" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="9.6328125" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="75.26953125" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="20.81640625" collapsed="false"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.6328125" collapsed="false"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="19.54296875" collapsed="false"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="18.90625" collapsed="false"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="14.7265625" collapsed="false"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="13.26953125" collapsed="false"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="15.81640625" collapsed="false"/>
+    <col min="24" max="24" customWidth="true" width="19.7265625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="16" customHeight="1" x14ac:dyDescent="0.35">
@@ -1902,7 +1906,9 @@
       <c r="O2" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="P2" s="12"/>
+      <c r="P2" t="s">
+        <v>239</v>
+      </c>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
@@ -3623,23 +3629,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1796875" customWidth="1"/>
-    <col min="10" max="10" width="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="58.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="35.0" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.1796875" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="44.1796875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="42.6328125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="58.453125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="31.0" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.36328125" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="46.1796875" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="17.1796875" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="35.0" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.08984375" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="26.7265625" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="10.81640625" collapsed="false"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="18.453125" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.08984375" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="58.453125" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="13.36328125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -3758,14 +3764,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.08984375" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.26953125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.36328125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="39.26953125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.81640625" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.453125" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="32.08984375" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.453125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updates for the UI Changes (#7)
</commit_message>
<xml_diff>
--- a/src/test/resources/data/sample.xlsx
+++ b/src/test/resources/data/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddSubsidy" sheetId="3" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="296">
   <si>
     <t>Subsidy Control Number</t>
   </si>
@@ -1419,7 +1419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1926,10 +1926,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2576,7 +2576,7 @@
       <c r="F17" s="14"/>
       <c r="G17" s="12"/>
       <c r="H17" s="13">
-        <v>43831</v>
+        <v>44562</v>
       </c>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -2611,7 +2611,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13">
-        <v>44197</v>
+        <v>43831</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
@@ -2638,7 +2638,9 @@
         <v>117</v>
       </c>
       <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
+      <c r="C19" s="17" t="s">
+        <v>16</v>
+      </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
@@ -2670,7 +2672,9 @@
         <v>118</v>
       </c>
       <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
+      <c r="C20" s="17" t="s">
+        <v>16</v>
+      </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
@@ -2702,7 +2706,9 @@
         <v>119</v>
       </c>
       <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
+      <c r="C21" s="17" t="s">
+        <v>16</v>
+      </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
@@ -2734,7 +2740,9 @@
         <v>122</v>
       </c>
       <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
+      <c r="C22" s="17" t="s">
+        <v>16</v>
+      </c>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>

</xml_diff>

<commit_message>
Updates to UI test data
</commit_message>
<xml_diff>
--- a/src/test/resources/data/sample.xlsx
+++ b/src/test/resources/data/sample.xlsx
@@ -16,7 +16,7 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">AwardDetails!$A$1:$Q$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">AwardDetails!$A$1:$Q$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="284">
   <si>
     <t>Subsidy Control Number</t>
   </si>
@@ -572,45 +572,15 @@
     <t>Spending Sector</t>
   </si>
   <si>
-    <t>SC10033</t>
-  </si>
-  <si>
     <t>USTD_036</t>
   </si>
   <si>
     <t>Beneficiary</t>
   </si>
   <si>
-    <t>Adam Wilson &amp; Sons LTD</t>
-  </si>
-  <si>
-    <t>SC230058</t>
-  </si>
-  <si>
-    <t>Medium Organisation</t>
-  </si>
-  <si>
     <t>Goods</t>
   </si>
   <si>
-    <t>Mining and quarrying</t>
-  </si>
-  <si>
-    <t>£500,000</t>
-  </si>
-  <si>
-    <t>Dumfries &amp; Galloway Council</t>
-  </si>
-  <si>
-    <t>££600,000 - £7,500,000</t>
-  </si>
-  <si>
-    <t>04 March 2018</t>
-  </si>
-  <si>
-    <t>SCOTLAND</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -731,15 +701,9 @@
     <t>Automation 003</t>
   </si>
   <si>
-    <t>Beatrice Offshore Wind Farm</t>
-  </si>
-  <si>
     <t>Automation 004</t>
   </si>
   <si>
-    <t>BEIS 2018 Call for CCUS Innovation</t>
-  </si>
-  <si>
     <t>Automation 005</t>
   </si>
   <si>
@@ -809,143 +773,143 @@
     <t>Organisation Size</t>
   </si>
   <si>
-    <t>Bus Emissions Abatement Retrofitting Scheme</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
+    <t>08 July 2019</t>
+  </si>
+  <si>
+    <t>10071517</t>
+  </si>
+  <si>
+    <t>West Midlands</t>
+  </si>
+  <si>
+    <t>Human health and social work activities</t>
+  </si>
+  <si>
+    <t>£2,000,001 - £5,000,000</t>
+  </si>
+  <si>
+    <t>11 August 2019</t>
+  </si>
+  <si>
+    <t>10778534</t>
+  </si>
+  <si>
+    <t>22 September 2019</t>
+  </si>
+  <si>
+    <t>123456784</t>
+  </si>
+  <si>
+    <t>Other service activities</t>
+  </si>
+  <si>
+    <t>Legal Basis</t>
+  </si>
+  <si>
+    <t>GA Websubsidy Link</t>
+  </si>
+  <si>
+    <t>South East</t>
+  </si>
+  <si>
+    <t>Water supply; sewerage, waste management and remediation activities</t>
+  </si>
+  <si>
+    <t>Guarantee</t>
+  </si>
+  <si>
+    <t>South West</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+  </si>
+  <si>
+    <t>Accommodation and food service activities</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>SC10129</t>
+  </si>
+  <si>
+    <t>BFI</t>
+  </si>
+  <si>
+    <t>Micro (fewer than 10 employees)</t>
+  </si>
+  <si>
+    <t>Small (between 10 and 49 employees)</t>
+  </si>
+  <si>
+    <t>Medium (between 50 and 249 employees)</t>
+  </si>
+  <si>
+    <t>Legal basis text</t>
+  </si>
+  <si>
+    <t>From 01 December 2021 to 01 January 2025</t>
+  </si>
+  <si>
+    <t>01 December 2021</t>
+  </si>
+  <si>
+    <t>https://www.google.com</t>
+  </si>
+  <si>
     <t>£800,000</t>
   </si>
   <si>
-    <t>Isle of Anglesey county council</t>
-  </si>
-  <si>
-    <t>08 July 2019</t>
-  </si>
-  <si>
-    <t>Micro organisation</t>
-  </si>
-  <si>
-    <t>10071517</t>
-  </si>
-  <si>
-    <t>West Midlands</t>
-  </si>
-  <si>
-    <t>Human health and social work activities</t>
-  </si>
-  <si>
-    <t>Business Growth Capital Grant Programme</t>
-  </si>
-  <si>
-    <t>£2,000,001 - £5,000,000</t>
-  </si>
-  <si>
-    <t>Norfolk County Council</t>
-  </si>
-  <si>
-    <t>11 August 2019</t>
-  </si>
-  <si>
-    <t>Small organisation</t>
-  </si>
-  <si>
-    <t>10778534</t>
-  </si>
-  <si>
-    <t>Capital allowances: extension of enhanced capital allowances for car and goods vehicles to 2018</t>
-  </si>
-  <si>
     <t>£1,000,000</t>
   </si>
   <si>
-    <t>Flintshire County council</t>
-  </si>
-  <si>
-    <t>22 September 2019</t>
-  </si>
-  <si>
-    <t>123456784</t>
-  </si>
-  <si>
-    <t>Other service activities</t>
-  </si>
-  <si>
-    <t>Legal Basis</t>
-  </si>
-  <si>
-    <t>GA Websubsidy Link</t>
-  </si>
-  <si>
-    <t>SC10007</t>
-  </si>
-  <si>
-    <t>South East</t>
-  </si>
-  <si>
-    <t>Water supply; sewerage, waste management and remediation activities</t>
-  </si>
-  <si>
-    <t>https://ec.europa.eu/competition/state_aid/cases/273717/273717_1970405_10_1.pdf</t>
-  </si>
-  <si>
-    <t>Guarantee</t>
-  </si>
-  <si>
-    <t>From 13 August 2018 to 31 March 2023</t>
-  </si>
-  <si>
-    <t>13 August 2018</t>
-  </si>
-  <si>
-    <t>SC10008</t>
-  </si>
-  <si>
-    <t>South West</t>
-  </si>
-  <si>
-    <t>Infrastructure</t>
-  </si>
-  <si>
-    <t>Accommodation and food service activities</t>
-  </si>
-  <si>
-    <t>https://ec.europa.eu/competition/state_aid/cases/253214/253214_1583639_82_2.pdf</t>
-  </si>
-  <si>
-    <t>From 31 March 2018 to 28 March 2033</t>
-  </si>
-  <si>
-    <t>31 March 2018</t>
-  </si>
-  <si>
-    <t>SC10009</t>
+    <t>COVID19 Relief</t>
+  </si>
+  <si>
+    <t>SC10130</t>
+  </si>
+  <si>
+    <t>Ad Hoc Case</t>
+  </si>
+  <si>
+    <t>From 01 January 2022 to 01 January 2022</t>
+  </si>
+  <si>
+    <t>01 January 2022</t>
+  </si>
+  <si>
+    <t>Student Learning Support</t>
+  </si>
+  <si>
+    <t>SC10126</t>
+  </si>
+  <si>
+    <t>www.studentslearningsupport.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direct Grant </t>
+  </si>
+  <si>
+    <t>From 01 March 2021 to 01 March 2023</t>
+  </si>
+  <si>
+    <t>01 March 2021</t>
   </si>
   <si>
     <t>Scotland</t>
   </si>
   <si>
     <t>Information and communication</t>
-  </si>
-  <si>
-    <t>Transport Act, Railways Act, Scotland Act</t>
-  </si>
-  <si>
-    <t>https://ec.europa.eu/competition/state_aid/cases1/202010/284923_2136865_11_1.pdf</t>
-  </si>
-  <si>
-    <t>From 01 April 2019 to 31 March 2021</t>
-  </si>
-  <si>
-    <t>01 April 2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -978,13 +942,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -1035,9 +992,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1091,9 +1048,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1103,19 +1057,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1420,7 +1373,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1926,10 +1879,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1948,7 +1901,7 @@
     <col min="12" max="14" width="19.7265625" customWidth="1"/>
     <col min="15" max="15" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="75.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18.6328125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="32.6328125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18.90625" bestFit="1" customWidth="1"/>
@@ -2050,7 +2003,7 @@
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="O2" s="18" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
@@ -2069,16 +2022,16 @@
         <v>121</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>90</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>91</v>
@@ -2112,7 +2065,7 @@
         <v>89</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
@@ -2130,7 +2083,7 @@
         <v>136</v>
       </c>
       <c r="P4" s="16" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
@@ -2146,7 +2099,7 @@
         <v>98</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
@@ -2164,7 +2117,7 @@
         <v>136</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
@@ -2179,8 +2132,8 @@
       <c r="A6" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>202</v>
+      <c r="B6" s="26" t="s">
+        <v>259</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
@@ -2198,7 +2151,7 @@
         <v>136</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>199</v>
+        <v>220</v>
       </c>
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
@@ -2252,7 +2205,7 @@
         <v>93</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
@@ -2271,7 +2224,7 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
       <c r="S8" s="16" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="T8" s="15"/>
       <c r="U8" s="15"/>
@@ -2288,7 +2241,7 @@
         <v>93</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -2307,7 +2260,7 @@
       <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
       <c r="S9" s="16" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="T9" s="15"/>
       <c r="U9" s="15"/>
@@ -2323,8 +2276,8 @@
       <c r="C10" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>202</v>
+      <c r="D10" s="26" t="s">
+        <v>192</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -2343,7 +2296,7 @@
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
       <c r="S10" s="16" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="T10" s="15"/>
       <c r="U10" s="15"/>
@@ -2431,7 +2384,7 @@
         <v>93</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
@@ -2448,7 +2401,7 @@
       <c r="R13" s="15"/>
       <c r="S13" s="15"/>
       <c r="T13" s="16" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="U13" s="15"/>
       <c r="V13" s="15"/>
@@ -2467,7 +2420,7 @@
         <v>93</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -2484,7 +2437,7 @@
       <c r="R14" s="15"/>
       <c r="S14" s="15"/>
       <c r="T14" s="16" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="U14" s="15"/>
       <c r="V14" s="15"/>
@@ -2502,8 +2455,8 @@
       <c r="F15" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="27" t="s">
-        <v>211</v>
+      <c r="G15" s="26" t="s">
+        <v>201</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -2520,7 +2473,7 @@
       <c r="R15" s="15"/>
       <c r="S15" s="15"/>
       <c r="T15" s="16" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="U15" s="15"/>
       <c r="V15" s="15"/>
@@ -2576,7 +2529,7 @@
       <c r="F17" s="14"/>
       <c r="G17" s="12"/>
       <c r="H17" s="13">
-        <v>44562</v>
+        <v>44197</v>
       </c>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -2594,7 +2547,7 @@
       <c r="T17" s="15"/>
       <c r="U17" s="15"/>
       <c r="V17" s="13">
-        <v>43466</v>
+        <v>44197</v>
       </c>
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
@@ -2638,8 +2591,8 @@
         <v>117</v>
       </c>
       <c r="B19" s="16"/>
-      <c r="C19" s="17" t="s">
-        <v>16</v>
+      <c r="C19" t="s">
+        <v>92</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -2672,8 +2625,8 @@
         <v>118</v>
       </c>
       <c r="B20" s="16"/>
-      <c r="C20" s="17" t="s">
-        <v>16</v>
+      <c r="C20" t="s">
+        <v>92</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -2782,16 +2735,16 @@
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
       <c r="J23" s="12" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
       <c r="N23" s="12"/>
       <c r="O23" s="18" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="P23" s="12"/>
       <c r="Q23" s="15"/>
@@ -2853,7 +2806,7 @@
         <v>93</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L25" s="16"/>
       <c r="M25" s="12"/>
@@ -2865,7 +2818,7 @@
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
       <c r="S25" s="16" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="T25" s="16"/>
       <c r="U25" s="15"/>
@@ -2889,7 +2842,7 @@
         <v>93</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="L26" s="16"/>
       <c r="M26" s="12"/>
@@ -2901,7 +2854,7 @@
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
       <c r="S26" s="16" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="T26" s="16"/>
       <c r="U26" s="15"/>
@@ -2924,12 +2877,12 @@
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
       <c r="L27" s="12" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
       <c r="O27" s="18" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="P27" s="12"/>
       <c r="Q27" s="15"/>
@@ -2956,7 +2909,7 @@
       <c r="J28" s="16"/>
       <c r="K28" s="16"/>
       <c r="L28" s="12" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="M28" s="16"/>
       <c r="N28" s="16"/>
@@ -2968,7 +2921,7 @@
       <c r="R28" s="15"/>
       <c r="T28" s="15"/>
       <c r="U28" s="12" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="V28" s="15"/>
       <c r="W28" s="15"/>
@@ -2990,13 +2943,13 @@
       <c r="K29" s="16"/>
       <c r="L29" s="16"/>
       <c r="M29" s="12" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="N29" s="16" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="O29" s="18" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="P29" s="12"/>
       <c r="Q29" s="15"/>
@@ -3024,7 +2977,7 @@
       <c r="K30" s="16"/>
       <c r="L30" s="16"/>
       <c r="M30" s="12" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="N30" s="16"/>
       <c r="O30" s="18" t="s">
@@ -3035,7 +2988,7 @@
       <c r="R30" s="15"/>
       <c r="S30" s="15"/>
       <c r="T30" s="12" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="U30" s="16"/>
       <c r="V30" s="15"/>
@@ -3061,7 +3014,7 @@
         <v>93</v>
       </c>
       <c r="N31" s="16" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="O31" s="18" t="s">
         <v>126</v>
@@ -3071,7 +3024,7 @@
       <c r="R31" s="15"/>
       <c r="S31" s="15"/>
       <c r="T31" s="16" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="U31" s="16"/>
       <c r="V31" s="15"/>
@@ -3097,7 +3050,7 @@
         <v>93</v>
       </c>
       <c r="N32" s="16" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="O32" s="18" t="s">
         <v>126</v>
@@ -3107,7 +3060,7 @@
       <c r="R32" s="15"/>
       <c r="S32" s="15"/>
       <c r="T32" s="16" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="U32" s="16"/>
       <c r="V32" s="15"/>
@@ -3119,17 +3072,17 @@
         <v>159</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="13">
@@ -3185,7 +3138,7 @@
         <v>160</v>
       </c>
       <c r="P34" s="16"/>
-      <c r="Q34" s="15"/>
+      <c r="Q34" s="16"/>
       <c r="R34" s="15"/>
       <c r="S34" s="15"/>
       <c r="T34" s="15"/>
@@ -3199,7 +3152,7 @@
         <v>162</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C35" s="16"/>
       <c r="D35" s="16"/>
@@ -3214,11 +3167,11 @@
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
       <c r="O35" s="18" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="P35" s="16"/>
-      <c r="Q35" s="15" t="s">
-        <v>66</v>
+      <c r="Q35" s="16" t="s">
+        <v>271</v>
       </c>
       <c r="R35" s="15"/>
       <c r="S35" s="15"/>
@@ -3233,7 +3186,7 @@
         <v>168</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -3248,11 +3201,11 @@
       <c r="M36" s="16"/>
       <c r="N36" s="16"/>
       <c r="O36" s="18" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="P36" s="16"/>
-      <c r="Q36" s="15" t="s">
-        <v>226</v>
+      <c r="Q36" s="8" t="s">
+        <v>276</v>
       </c>
       <c r="R36" s="15"/>
       <c r="S36" s="15"/>
@@ -3264,10 +3217,10 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -3282,11 +3235,11 @@
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
       <c r="O37" s="18" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="P37" s="16"/>
       <c r="Q37" s="15" t="s">
-        <v>228</v>
+        <v>66</v>
       </c>
       <c r="R37" s="15"/>
       <c r="S37" s="15"/>
@@ -3298,18 +3251,18 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
       <c r="J38" s="16"/>
       <c r="K38" s="16"/>
       <c r="L38" s="16"/>
@@ -3318,8 +3271,8 @@
       <c r="O38" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="P38" s="28" t="s">
-        <v>229</v>
+      <c r="P38" s="27" t="s">
+        <v>217</v>
       </c>
       <c r="Q38" s="15"/>
       <c r="R38" s="15"/>
@@ -3332,18 +3285,18 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
       <c r="J39" s="16"/>
       <c r="K39" s="16"/>
       <c r="L39" s="16"/>
@@ -3352,8 +3305,8 @@
       <c r="O39" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="P39" s="28" t="s">
-        <v>230</v>
+      <c r="P39" s="27" t="s">
+        <v>218</v>
       </c>
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
@@ -3366,18 +3319,18 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
       <c r="J40" s="16"/>
       <c r="K40" s="16"/>
       <c r="L40" s="16"/>
@@ -3386,8 +3339,8 @@
       <c r="O40" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="P40" s="28" t="s">
-        <v>231</v>
+      <c r="P40" s="27" t="s">
+        <v>219</v>
       </c>
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
@@ -3400,10 +3353,10 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>52</v>
@@ -3429,7 +3382,7 @@
         <v>136</v>
       </c>
       <c r="P41" s="12" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
@@ -3442,10 +3395,10 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>52</v>
@@ -3473,7 +3426,7 @@
         <v>136</v>
       </c>
       <c r="P42" s="12" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="Q42" s="15"/>
       <c r="R42" s="15"/>
@@ -3486,7 +3439,7 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>85</v>
@@ -3517,7 +3470,7 @@
         <v>136</v>
       </c>
       <c r="P43" s="12" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
@@ -3530,13 +3483,13 @@
     </row>
     <row r="44" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="12" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>85</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="12" t="s">
@@ -3561,7 +3514,7 @@
         <v>136</v>
       </c>
       <c r="P44" s="12" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
@@ -3574,7 +3527,7 @@
     </row>
     <row r="45" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="12" t="s">
@@ -3582,7 +3535,7 @@
       </c>
       <c r="D45" s="12"/>
       <c r="E45" s="12" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="F45" s="12" t="s">
         <v>17</v>
@@ -3603,7 +3556,7 @@
         <v>136</v>
       </c>
       <c r="P45" s="12" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="Q45" s="15"/>
       <c r="R45" s="15"/>
@@ -3616,7 +3569,7 @@
     </row>
     <row r="46" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="12" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="B46" s="12"/>
       <c r="C46" s="12" t="s">
@@ -3645,7 +3598,7 @@
         <v>136</v>
       </c>
       <c r="P46" s="12" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
@@ -3672,7 +3625,7 @@
       <c r="M47" s="13"/>
       <c r="N47" s="13"/>
       <c r="O47" s="19" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="P47" s="14"/>
       <c r="Q47" s="15"/>
@@ -3700,7 +3653,7 @@
       <c r="M48" s="13"/>
       <c r="N48" s="13"/>
       <c r="O48" s="19" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="P48" s="14"/>
       <c r="Q48" s="15"/>
@@ -3902,7 +3855,7 @@
       <c r="X58" s="8"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" showErrorMessage="1" errorTitle="Automation" error="Do not change the Column header name as this will break Automation scripts" prompt="Do not change the Column Header Values" sqref="B1">
       <formula1>"Recipient"</formula1>
     </dataValidation>
@@ -3914,67 +3867,69 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="44.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="42.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="58.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.1796875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="26.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="58.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="42.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="36.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="26.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.6328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="34.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="C1" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="D1" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="E1" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="F1" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="G1" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="H1" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="I1" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="J1" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="M1" t="s">
         <v>6</v>
@@ -3994,99 +3949,99 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2717</v>
-      </c>
-      <c r="D2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" s="7">
+        <v>20828</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>253</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>254</v>
+        <v>240</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>269</v>
       </c>
       <c r="I2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="K2" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="L2" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="M2" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="30" t="s">
-        <v>258</v>
+      <c r="N2" s="28" t="s">
+        <v>242</v>
       </c>
       <c r="O2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P2" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="Q2" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>230</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2718</v>
-      </c>
-      <c r="D3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" s="7">
+        <v>20829</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>245</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="I3" t="s">
         <v>261</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>262</v>
-      </c>
-      <c r="H3" t="s">
-        <v>253</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>246</v>
+      </c>
+      <c r="K3" t="s">
+        <v>218</v>
+      </c>
+      <c r="L3" t="s">
         <v>263</v>
-      </c>
-      <c r="J3" t="s">
-        <v>264</v>
-      </c>
-      <c r="K3" t="s">
-        <v>230</v>
-      </c>
-      <c r="L3" t="s">
-        <v>265</v>
       </c>
       <c r="M3" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="30" t="s">
-        <v>266</v>
+      <c r="N3" s="28" t="s">
+        <v>247</v>
       </c>
       <c r="O3" t="s">
         <v>24</v>
@@ -4095,110 +4050,60 @@
         <v>25</v>
       </c>
       <c r="Q3" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>231</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2719</v>
-      </c>
-      <c r="D4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" s="7">
+        <v>20830</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F4" t="s">
-        <v>190</v>
+      <c r="F4" s="7" t="s">
+        <v>180</v>
       </c>
       <c r="G4" t="s">
-        <v>253</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>268</v>
+        <v>240</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>270</v>
       </c>
       <c r="I4" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="J4" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="K4" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="L4" t="s">
-        <v>39</v>
+        <v>264</v>
       </c>
       <c r="M4" t="s">
         <v>27</v>
       </c>
       <c r="N4" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="O4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P4" t="s">
         <v>70</v>
       </c>
       <c r="Q4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="B5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" t="s">
-        <v>183</v>
-      </c>
-      <c r="H5" t="s">
-        <v>181</v>
-      </c>
-      <c r="I5" t="s">
-        <v>182</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="K5" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="L5" t="s">
-        <v>178</v>
-      </c>
-      <c r="M5" t="s">
-        <v>60</v>
-      </c>
-      <c r="N5" t="s">
-        <v>177</v>
-      </c>
-      <c r="O5" t="s">
-        <v>179</v>
-      </c>
-      <c r="P5" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>180</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -4211,7 +4116,7 @@
           <x14:formula1>
             <xm:f>'C:\Users\321020\Desktop\BU\[BU Auto Master Latest.xlsx]Dropdown'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:Q4 L2:M4</xm:sqref>
+          <xm:sqref>M2:M4 O2:P4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4224,19 +4129,22 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="39.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -4244,7 +4152,7 @@
         <v>166</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>163</v>
@@ -4256,10 +4164,10 @@
         <v>115</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>273</v>
+        <v>251</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>274</v>
+        <v>252</v>
       </c>
       <c r="H1" s="24" t="s">
         <v>126</v>
@@ -4274,116 +4182,116 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>276</v>
+        <v>260</v>
+      </c>
+      <c r="C2" t="s">
+        <v>282</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>277</v>
+        <v>52</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>283</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>278</v>
+        <v>265</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>268</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>279</v>
+        <v>35</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>167</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>226</v>
+        <v>271</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>283</v>
+        <v>253</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>285</v>
+        <v>92</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>254</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>286</v>
+        <v>265</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>268</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>53</v>
+        <v>255</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>167</v>
+        <v>273</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="K3" s="34" t="s">
-        <v>288</v>
+        <v>274</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>228</v>
+        <v>276</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>290</v>
+        <v>256</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>52</v>
+        <v>257</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>291</v>
+        <v>258</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>293</v>
+        <v>265</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>278</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>35</v>
+        <v>279</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>167</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="K4" s="33" t="s">
-        <v>295</v>
+        <v>280</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G4" r:id="rId2"/>
-    <hyperlink ref="G3" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>